<commit_message>
Route finding partially working: tests need some revision
</commit_message>
<xml_diff>
--- a/MazeLayout.xlsx
+++ b/MazeLayout.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry_000\Documents\School\CSCI 306\FinalProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
@@ -113,6 +118,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -160,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -195,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,15 +412,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="22" max="22" width="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -476,8 +487,11 @@
       <c r="U1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -541,8 +555,11 @@
       <c r="U2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -606,8 +623,11 @@
       <c r="U3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -671,8 +691,11 @@
       <c r="U4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -736,8 +759,11 @@
       <c r="U5" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -801,8 +827,11 @@
       <c r="U6" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -866,8 +895,11 @@
       <c r="U7" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -931,8 +963,11 @@
       <c r="U8" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -996,8 +1031,11 @@
       <c r="U9" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1061,8 +1099,11 @@
       <c r="U10" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1126,8 +1167,11 @@
       <c r="U11" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1191,8 +1235,11 @@
       <c r="U12" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1256,8 +1303,11 @@
       <c r="U13" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1321,8 +1371,11 @@
       <c r="U14" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1386,8 +1439,11 @@
       <c r="U15" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1451,8 +1507,11 @@
       <c r="U16" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1516,8 +1575,11 @@
       <c r="U17" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>1</v>
       </c>
@@ -1581,8 +1643,11 @@
       <c r="U18" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1646,8 +1711,11 @@
       <c r="U19" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -1710,6 +1778,74 @@
       </c>
       <c r="U20" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="V20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+      <c r="J21">
+        <v>9</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>11</v>
+      </c>
+      <c r="M21">
+        <v>12</v>
+      </c>
+      <c r="N21">
+        <v>13</v>
+      </c>
+      <c r="O21">
+        <v>14</v>
+      </c>
+      <c r="P21">
+        <v>15</v>
+      </c>
+      <c r="Q21">
+        <v>16</v>
+      </c>
+      <c r="R21">
+        <v>17</v>
+      </c>
+      <c r="S21">
+        <v>18</v>
+      </c>
+      <c r="T21">
+        <v>19</v>
+      </c>
+      <c r="U21">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>